<commit_message>
for now html files
</commit_message>
<xml_diff>
--- a/Excel Functions.xlsx
+++ b/Excel Functions.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Functions" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,9 +25,148 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+  <si>
+    <t>returns number of numerical values in a data range</t>
+  </si>
+  <si>
+    <t>SlNo</t>
+  </si>
+  <si>
+    <t>COUNT(A:A)</t>
+  </si>
+  <si>
+    <t>https://gmail.com</t>
+  </si>
+  <si>
+    <t>HYPERLINK(Sheet1!A1,"Gmail")</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>Function syntax</t>
+  </si>
+  <si>
+    <t>tooltip</t>
+  </si>
+  <si>
+    <t>Just type the complete hyperlink as shown in A4 cell and right-click on it to select 'Edit Hyperlink'. In the properties window, you can type the actual website address or a place in the current file</t>
+  </si>
+  <si>
+    <t>EOMONTH("27-9-2022",1)
+EOMONTH("27-9-2022",-2)</t>
+  </si>
+  <si>
+    <t>It returns the last date after adding months indicated by 2nd parameter</t>
+  </si>
+  <si>
+    <t>This hyperlink() has first parameter pointing to a cell value that has web address. The second parameter is an alias name</t>
+  </si>
+  <si>
+    <t>EDATE("27-09-2022",-1)</t>
+  </si>
+  <si>
+    <t>Returns the date after adding the number of months indicated by second parameter. A negative 2nd paramter indicates that the specified date minus the months specified.</t>
+  </si>
+  <si>
+    <t>Oranges</t>
+  </si>
+  <si>
+    <t>Grapes</t>
+  </si>
+  <si>
+    <t>Banana</t>
+  </si>
+  <si>
+    <t>mangoes</t>
+  </si>
+  <si>
+    <t>CHOOSE(2,Sheet1!E1,Sheet1!E2,Sheet1!E3,Sheet1!E4)
+CHOOSE(4,"Red","green","yellow","black")</t>
+  </si>
+  <si>
+    <t>First parameter is the index or position number. The rest of the parameters should be discrete cell values. Never use a range of cells.</t>
+  </si>
+  <si>
+    <t>DAY(NOW()),DAY("15-10-2022")</t>
+  </si>
+  <si>
+    <t>IFNA(VLOOKUP(23,Sheet1!A1:A5,0),"no value found")</t>
+  </si>
+  <si>
+    <t>Returns the day from the given date value</t>
+  </si>
+  <si>
+    <t>In this example if the Vlookup function is not yeilding any value, then 2nd parameter is returned</t>
+  </si>
+  <si>
+    <t>Returns the ascii value of first character of the string provided</t>
+  </si>
+  <si>
+    <t>CODE("sri")</t>
+  </si>
+  <si>
+    <t>Returns the character of an ascii value</t>
+  </si>
+  <si>
+    <t>CHAR(97)</t>
+  </si>
+  <si>
+    <t>returns non printable characters. It removes even carriage returns. If there are 2 or more lines where new line carriage returns are not printeed</t>
+  </si>
+  <si>
+    <t>CLEAN(B5)</t>
+  </si>
+  <si>
+    <t>DOLLAR(23.56,3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adds a currency symbol along with decimals as specified by 2nd parameter </t>
+  </si>
+  <si>
+    <t>case sensitive function</t>
+  </si>
+  <si>
+    <t>not a case sensitive function</t>
+  </si>
+  <si>
+    <t>FIND("last",D5)</t>
+  </si>
+  <si>
+    <t>SEARCH("LAST",D5)</t>
+  </si>
+  <si>
+    <t>FIXED(Sheet1!A5,1,TRUE)</t>
+  </si>
+  <si>
+    <t>rounding off to nearest decimal. The 3rd parameter will remove or keeps commas in the number provided in first argument</t>
+  </si>
+  <si>
+    <t>LEN(B11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yields length of the </t>
+  </si>
+  <si>
+    <t>CONCATENATE(A1,A2)</t>
+  </si>
+  <si>
+    <t>Never give a range. Indicidual cell references are to be given</t>
+  </si>
+  <si>
+    <t>TEXT(Sheet1!A8,"dd mmm yyyy")</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$USD]\ #,##0.00"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -34,16 +174,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF098658"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -51,14 +211,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -337,24 +542,372 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>1223456.8959999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>44833</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1">
+        <f>COUNT(A:A)</f>
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6" t="str">
+        <f>HYPERLINK(Sheet1!A1,"Gmail")</f>
+        <v>Gmail</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7">
+        <f>EOMONTH("27-09-2022",0)</f>
+        <v>44834</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="7">
+        <f>EDATE("27-09-2022",-1)</f>
+        <v>44800</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="str">
+        <f>CHOOSE(2,Sheet1!E1,Sheet1!E2,Sheet1!E3,Sheet1!E4)</f>
+        <v>Grapes</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(23,Sheet1!A1:A5,0),"no value found")</f>
+        <v>no value found</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1">
+        <f>CODE("sri")</f>
+        <v>115</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f>CHAR(97)</f>
+        <v>a</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="str">
+        <f>CLEAN(B5)</f>
+        <v>EOMONTH("27-9-2022",1)EOMONTH("27-9-2022",-2)</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>12</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="10" t="str">
+        <f>DOLLAR(23.56,3)</f>
+        <v>₹ 23.560</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14">
+        <f>FIND("last",D5)</f>
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15">
+        <f>SEARCH("LAST",D5)</f>
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="str">
+        <f>FIXED(Sheet1!A5,1,TRUE)</f>
+        <v>1223456.9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="str">
+        <f>CONCATENATE(A1,A2)</f>
+        <v>SlNo1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="str">
+        <f>TEXT(Sheet1!A8,"dd mmm yyyy")</f>
+        <v>29 Sep 2022</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="12">
+        <f>12+34+56+78</f>
+        <v>180</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>